<commit_message>
Fixed operational issues regarding deadheads, cleaned the list of controllers, added sorting to stat sections, and changed to store data as numbers to allow graphing
</commit_message>
<xml_diff>
--- a/Source/Files/Template.xlsx
+++ b/Source/Files/Template.xlsx
@@ -138,9 +138,6 @@
     <t>(Amps RMS)</t>
   </si>
   <si>
-    <t>RPM</t>
-  </si>
-  <si>
     <t>(Percent)</t>
   </si>
   <si>
@@ -148,12 +145,18 @@
   </si>
   <si>
     <t>Desired Parameters</t>
+  </si>
+  <si>
+    <t>(RPM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -322,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -349,6 +352,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -364,19 +391,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -386,9 +401,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -711,7 +723,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="13.7109375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="11" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" style="10" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="9" customWidth="1"/>
+    <col min="8" max="9" width="13.7109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="11" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" style="9" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
     <col min="13" max="14" width="26.7109375" style="9" customWidth="1"/>
@@ -719,123 +737,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="15"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
       <c r="M1" s="4" t="s">
         <v>23</v>
       </c>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="23" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="15"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="23" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="23" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="15"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
       <c r="M3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
       <c r="M4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="15"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="15"/>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="15"/>
@@ -847,38 +865,38 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="26"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="29"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="29"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -937,7 +955,7 @@
         <v>29</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1">
@@ -959,14 +977,14 @@
       <c r="F10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>21</v>
@@ -986,24 +1004,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A6:B7"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="A4:B4"/>
@@ -1018,6 +1018,24 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="C6:N7"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1034,7 +1052,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="10" width="13.7109375" style="9" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="11" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" style="10" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" style="11" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="9" customWidth="1"/>
+    <col min="8" max="9" width="13.7109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="11" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" style="9" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
     <col min="13" max="14" width="26.7109375" style="9" customWidth="1"/>
@@ -1042,123 +1066,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="15"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="19"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
       <c r="M1" s="7" t="s">
         <v>23</v>
       </c>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="23" t="s">
+      <c r="B2" s="17"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="15"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="23" t="s">
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="14" t="s">
         <v>14</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="7" t="s">
         <v>24</v>
       </c>
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="23" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="15"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
       <c r="M3" s="6" t="s">
         <v>21</v>
       </c>
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="19" t="s">
+      <c r="B4" s="23"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="19"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="21" t="s">
+      <c r="F4" s="17"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
       <c r="M4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="15"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="15"/>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="F5" s="15"/>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="J5" s="15"/>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="22" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="15"/>
@@ -1170,38 +1194,38 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="26"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="29"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="29"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="32"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -1260,7 +1284,7 @@
         <v>29</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1">
@@ -1282,14 +1306,14 @@
       <c r="F10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>41</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>42</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>21</v>
@@ -1309,18 +1333,9 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="C6:N7"/>
     <mergeCell ref="K4:L4"/>
@@ -1338,9 +1353,18 @@
     <mergeCell ref="A6:B7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1359,7 +1383,11 @@
   <cols>
     <col min="1" max="1" width="16.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" customWidth="1"/>
-    <col min="3" max="9" width="13.7109375" style="9" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="11" customWidth="1"/>
+    <col min="6" max="7" width="13.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="9" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="11" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" customWidth="1"/>
     <col min="11" max="12" width="16.7109375" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Still in the process of adding a sheet to the output excel file meant for printing now that all sheets are being locked
</commit_message>
<xml_diff>
--- a/Source/Files/Template.xlsx
+++ b/Source/Files/Template.xlsx
@@ -10,13 +10,14 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Statistics" sheetId="4" r:id="rId2"/>
     <sheet name="Profile" sheetId="3" r:id="rId3"/>
+    <sheet name="Printable" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="43">
   <si>
     <t>Serial Numbers</t>
   </si>
@@ -39,12 +40,6 @@
     <t>Command</t>
   </si>
   <si>
-    <t>Voltage Reading</t>
-  </si>
-  <si>
-    <t>Pump</t>
-  </si>
-  <si>
     <t>CA Number</t>
   </si>
   <si>
@@ -148,6 +143,9 @@
   </si>
   <si>
     <t>(RPM)</t>
+  </si>
+  <si>
+    <t>Page 1 of 1</t>
   </si>
 </sst>
 </file>
@@ -157,7 +155,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +166,36 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -325,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,6 +392,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,6 +458,87 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -737,166 +856,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="17" t="s">
+      <c r="J1" s="21"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="17" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="8"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="17" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
+      <c r="J2" s="19"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="8"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="17" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="17" t="s">
+      <c r="J3" s="19"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="23" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25" t="s">
+      <c r="J4" s="30"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="32"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="36"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -916,7 +1035,7 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>2</v>
@@ -928,78 +1047,78 @@
         <v>4</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="M9" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="G10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="J10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1066,166 +1185,166 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="17" t="s">
+      <c r="J1" s="21"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="17" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="17"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="8"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="17" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
+      <c r="J2" s="19"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N2" s="8"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="17" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="17" t="s">
+      <c r="J3" s="19"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="14" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="23" t="s">
+      <c r="F4" s="21"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="25" t="s">
+      <c r="J4" s="30"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="8"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="26"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="8"/>
-    </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="15"/>
-      <c r="I5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="29"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="33"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="32"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="36"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -1245,7 +1364,7 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" thickBot="1">
       <c r="A9" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>2</v>
@@ -1257,78 +1376,78 @@
         <v>4</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>30</v>
-      </c>
       <c r="M9" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1">
       <c r="A10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="G10" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="I10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="J10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1338,18 +1457,17 @@
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="C6:N7"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A6:B7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
@@ -1365,6 +1483,7 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K4:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1373,68 +1492,574 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="4" width="13.7109375" style="9" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="11" customWidth="1"/>
     <col min="6" max="7" width="13.7109375" style="10" customWidth="1"/>
     <col min="8" max="8" width="13.7109375" style="9" customWidth="1"/>
     <col min="9" max="9" width="13.7109375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="11" max="12" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="14" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="21"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="13"/>
+    </row>
+    <row r="2" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="19"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="19"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="21"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="19"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="13"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="33"/>
+    </row>
+    <row r="7" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="36"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1">
+      <c r="A8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
+      <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="16.5" thickTop="1" thickBot="1"/>
-    <row r="3" spans="1:12" ht="16.5" thickTop="1" thickBot="1">
-      <c r="K3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="K9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickTop="1"/>
+    <row r="10" spans="1:14" ht="15.75" thickTop="1"/>
   </sheetData>
+  <mergeCells count="32">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:N7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" customHeight="1"/>
+  <cols>
+    <col min="1" max="10" width="10.7109375" style="16" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="16" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A1" s="51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="54"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="54"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+    </row>
+    <row r="2" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A2" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="54"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="51" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="52"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+    </row>
+    <row r="3" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A3" s="54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="54"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="54"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="51" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="52"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+    </row>
+    <row r="4" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A4" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="54"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="54"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="38"/>
+      <c r="K4" s="55"/>
+      <c r="L4" s="55"/>
+    </row>
+    <row r="5" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A5" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="52"/>
+      <c r="C5" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="52"/>
+      <c r="G5" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="52"/>
+      <c r="I5" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="52"/>
+      <c r="K5" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="48"/>
+    </row>
+    <row r="6" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A6" s="37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="38"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="52"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="60"/>
+      <c r="I6" s="56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="52"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="50"/>
+    </row>
+    <row r="7" spans="1:12" ht="11.25" customHeight="1">
+      <c r="A7" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="38"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
+    </row>
+    <row r="8" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A8" s="39"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="46"/>
+    </row>
+    <row r="9" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A9" s="61"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+    </row>
+    <row r="10" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A10" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="62" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
+      <c r="A11" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="62" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="63" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="63" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="37">
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A7:B8"/>
+    <mergeCell ref="C7:L8"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More changes to PC then rewrite some of RT to subVIs to clean up code
</commit_message>
<xml_diff>
--- a/Source/Files/Template.xlsx
+++ b/Source/Files/Template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Statistics" sheetId="4" r:id="rId2"/>
     <sheet name="Profile" sheetId="3" r:id="rId3"/>
-    <sheet name="Printable" sheetId="5" r:id="rId4"/>
+    <sheet name="For Printing" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -399,65 +399,89 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -465,6 +489,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -501,24 +528,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -530,15 +539,6 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -856,126 +856,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="21" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
       <c r="M1" s="4" t="s">
         <v>21</v>
       </c>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="21" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="21" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
       <c r="M4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="19"/>
+      <c r="A5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="25"/>
       <c r="M5" s="6" t="s">
         <v>19</v>
       </c>
@@ -984,38 +984,38 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="33"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="36"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="38"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -1123,6 +1123,24 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A6:B7"/>
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="A4:B4"/>
@@ -1137,24 +1155,6 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="C6:N7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1185,126 +1185,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="21" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
       <c r="M1" s="7" t="s">
         <v>21</v>
       </c>
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="7" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="21" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="21" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
       <c r="M4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="19"/>
+      <c r="A5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="25"/>
       <c r="M5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1313,38 +1313,38 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="33"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="36"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="38"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -1452,22 +1452,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="C6:N7"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
     <mergeCell ref="A6:B7"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
@@ -1484,6 +1468,22 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K4:L4"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="C6:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1514,126 +1514,126 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="21" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
       <c r="M1" s="14" t="s">
         <v>21</v>
       </c>
       <c r="N1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="18" t="s">
+      <c r="F2" s="25"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
       <c r="M2" s="14" t="s">
         <v>22</v>
       </c>
       <c r="N2" s="13"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="21" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18" t="s">
+      <c r="F3" s="29"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="19"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
       <c r="M3" s="6" t="s">
         <v>19</v>
       </c>
       <c r="N3" s="13"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="21" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="29" t="s">
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
       <c r="M4" s="6" t="s">
         <v>19</v>
       </c>
       <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="19"/>
-      <c r="I5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="19"/>
+      <c r="A5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="25"/>
+      <c r="C5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="25"/>
+      <c r="E5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="25"/>
+      <c r="I5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="25"/>
       <c r="M5" s="6" t="s">
         <v>19</v>
       </c>
@@ -1642,38 +1642,38 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="33"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="35"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="36"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37"/>
+      <c r="N7" s="38"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -1720,6 +1720,26 @@
     <row r="10" spans="1:14" ht="15.75" thickTop="1"/>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="C6:N7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="K2:L2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -1732,26 +1752,6 @@
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A6:B7"/>
-    <mergeCell ref="C6:N7"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="K5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1774,277 +1774,253 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="54"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="54" t="s">
+      <c r="F1" s="43"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="54"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
     </row>
     <row r="2" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="51" t="s">
+      <c r="B2" s="43"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="51" t="s">
+      <c r="F2" s="42"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="52"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
     </row>
     <row r="3" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="54"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="51" t="s">
+      <c r="F3" s="43"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="52"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="J3" s="42"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
     </row>
     <row r="4" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="54"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="54" t="s">
+      <c r="B4" s="43"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="54"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="37" t="s">
+      <c r="F4" s="43"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="38"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
     </row>
     <row r="5" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A5" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="52"/>
-      <c r="G5" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="52"/>
-      <c r="I5" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="52"/>
-      <c r="K5" s="47" t="s">
+      <c r="A5" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="42"/>
+      <c r="C5" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="42"/>
+      <c r="G5" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="42"/>
+      <c r="K5" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="L5" s="48"/>
+      <c r="L5" s="57"/>
     </row>
     <row r="6" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="57"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="51" t="s">
+      <c r="B6" s="46"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="52"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="56" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="52"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="50"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="42"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="59"/>
     </row>
     <row r="7" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="43"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="52"/>
     </row>
     <row r="8" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="46"/>
+      <c r="A8" s="48"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="54"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="55"/>
     </row>
     <row r="9" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A9" s="61"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
     </row>
     <row r="10" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A10" s="62" t="s">
+      <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="62" t="s">
+      <c r="C10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="62" t="s">
+      <c r="D10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="62" t="s">
+      <c r="E10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="62" t="s">
+      <c r="F10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="62" t="s">
+      <c r="G10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="62" t="s">
+      <c r="H10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="I10" s="62" t="s">
+      <c r="I10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="62" t="s">
+      <c r="J10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="62" t="s">
+      <c r="K10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L10" s="62" t="s">
+      <c r="L10" s="18" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A11" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="62" t="s">
+      <c r="A11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="62" t="s">
+      <c r="C11" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="62" t="s">
+      <c r="F11" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="62" t="s">
+      <c r="G11" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="H11" s="62" t="s">
+      <c r="H11" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I11" s="62" t="s">
+      <c r="I11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="K11" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="63" t="s">
+      <c r="J11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="19" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="A7:B8"/>
     <mergeCell ref="C7:L8"/>
@@ -2058,6 +2034,30 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:H6"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizing changes for next release, need to address why formatting from Excel template is not being kept in created files
</commit_message>
<xml_diff>
--- a/Source/Files/Template.xlsx
+++ b/Source/Files/Template.xlsx
@@ -350,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,6 +396,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -455,6 +466,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -527,22 +550,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,174 +864,169 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="9" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" style="8" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="7" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="72" customWidth="1"/>
+    <col min="2" max="10" width="13.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="72" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="72" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="7" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="20" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
       <c r="M1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="N1"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="60"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="16"/>
       <c r="N2"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="20" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
       <c r="M3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="20" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="F4" s="25"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="5"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="69"/>
       <c r="N4"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="18"/>
+      <c r="A5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="23"/>
       <c r="M5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="N5"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
       <c r="N6"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="40"/>
       <c r="N7"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
@@ -1165,174 +1179,169 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="7" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" style="9" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" style="8" customWidth="1"/>
-    <col min="5" max="6" width="13.7109375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="7" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" style="8" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="9" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" style="7" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="26.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" style="72" customWidth="1"/>
+    <col min="2" max="10" width="13.7109375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="72" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" style="72" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="7" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="20" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
       <c r="M1" s="6" t="s">
         <v>21</v>
       </c>
       <c r="N1"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="60"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="16"/>
       <c r="N2"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="20" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
       <c r="M3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="N3"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="20" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="F4" s="25"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="5"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="69"/>
       <c r="N4"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="18"/>
+      <c r="A5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="23"/>
       <c r="M5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="N5"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="32"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
       <c r="N6"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="35"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="40"/>
       <c r="N7"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
@@ -1487,170 +1496,172 @@
   <cols>
     <col min="1" max="1" width="13.7109375" style="7" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="4" width="13.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" style="9" customWidth="1"/>
-    <col min="6" max="7" width="13.7109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" style="7" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" style="9" customWidth="1"/>
-    <col min="10" max="12" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="18" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="9" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" style="8" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="18" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="19" customWidth="1"/>
+    <col min="11" max="12" width="13.7109375" customWidth="1"/>
     <col min="13" max="14" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="20" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="20" t="s">
+      <c r="F1" s="25"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="17" t="s">
+      <c r="J1" s="25"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="18"/>
+      <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="17" t="s">
+      <c r="F2" s="23"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="61"/>
-      <c r="N2" s="62"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="42"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="20" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="17" t="s">
+      <c r="F3" s="25"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="17" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="18"/>
+      <c r="N3" s="23"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="20" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="28" t="s">
+      <c r="F4" s="25"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="29"/>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="63"/>
-      <c r="N4" s="64"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="71"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="18"/>
-      <c r="I5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="18"/>
-      <c r="M5" s="63" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="64"/>
+      <c r="A5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="23"/>
+      <c r="I5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="23"/>
+      <c r="M5" s="43" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="44"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31"/>
-      <c r="M6" s="31"/>
-      <c r="N6" s="32"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="37"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="35"/>
+      <c r="A7" s="28"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
+      <c r="I7" s="39"/>
+      <c r="J7" s="39"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="39"/>
+      <c r="N7" s="40"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" thickBot="1">
       <c r="A8"/>
@@ -1661,12 +1672,13 @@
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
+      <c r="J8"/>
     </row>
     <row r="9" spans="1:14" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="18"/>
+      <c r="B9" s="23"/>
       <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1688,11 +1700,11 @@
       <c r="J9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="M9" s="18"/>
-      <c r="N9" s="65" t="s">
+      <c r="M9" s="23"/>
+      <c r="N9" s="17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1752,167 +1764,168 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" customHeight="1"/>
   <cols>
-    <col min="1" max="10" width="10.7109375" style="12" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="12" customWidth="1"/>
+    <col min="2" max="10" width="10.7109375" style="20" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" style="20" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" style="12" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="58" t="s">
+      <c r="B1" s="46"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="58"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="58" t="s">
+      <c r="F1" s="67"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="58"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="54" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="54" t="s">
+      <c r="F2" s="46"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
     </row>
     <row r="3" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="58" t="s">
+      <c r="B3" s="67"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="58"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="54" t="s">
+      <c r="F3" s="67"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="37"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
     </row>
     <row r="4" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="58" t="s">
+      <c r="B4" s="67"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="58"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="38" t="s">
+      <c r="F4" s="67"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="39"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
     </row>
     <row r="5" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A5" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="37"/>
-      <c r="I5" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="37"/>
-      <c r="K5" s="48" t="s">
+      <c r="A5" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="46"/>
+      <c r="E5" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="46"/>
+      <c r="G5" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="46"/>
+      <c r="I5" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="46"/>
+      <c r="K5" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="L5" s="49"/>
+      <c r="L5" s="58"/>
     </row>
     <row r="6" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="39"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54" t="s">
+      <c r="B6" s="48"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="37"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="51"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="46"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="60"/>
     </row>
     <row r="7" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="44"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
-      <c r="A8" s="40"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="47"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
+      <c r="L8" s="56"/>
     </row>
     <row r="9" spans="1:12" ht="11.25" customHeight="1" thickBot="1">
       <c r="A9" s="13"/>

</xml_diff>